<commit_message>
Erlach Napoleon Stalder Vater Welcker Radlof fertig
</commit_message>
<xml_diff>
--- a/Datasets/Erlach/Data/Erlach_JR.xlsx
+++ b/Datasets/Erlach/Data/Erlach_JR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julerickert/Documents/Akademie_Projekt/Datasets/Erlach/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F157D3-10F9-F54D-A166-84C5A3B4EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B49B89E-B1ED-124D-BA1F-D391BC64D77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{667C5683-ADBE-2B49-ACEF-B63231E960A4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2584" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2748" uniqueCount="510">
   <si>
     <t>ID</t>
   </si>
@@ -1563,6 +1563,9 @@
   </si>
   <si>
     <t>[Preußisch-Plattdeutsch] / Königsberg</t>
+  </si>
+  <si>
+    <t>Vergleich</t>
   </si>
 </sst>
 </file>
@@ -1980,11 +1983,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DB7810F-2200-2649-9C2C-F3C9823F050E}">
-  <dimension ref="A1:XFA169"/>
+  <dimension ref="A1:XFB169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W63" sqref="W63"/>
+      <selection pane="bottomLeft" activeCell="X2" sqref="X2:X164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1999,17 +2002,17 @@
     <col min="13" max="13" width="15.33203125" customWidth="1"/>
     <col min="14" max="15" width="12" customWidth="1"/>
     <col min="22" max="22" width="28.5" customWidth="1"/>
-    <col min="26" max="26" width="13.1640625" customWidth="1"/>
-    <col min="27" max="27" width="13" customWidth="1"/>
-    <col min="28" max="28" width="10.83203125" style="9"/>
-    <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="25" customWidth="1"/>
-    <col min="34" max="34" width="24.33203125" customWidth="1"/>
-    <col min="35" max="35" width="14.6640625" customWidth="1"/>
+    <col min="27" max="27" width="13.1640625" customWidth="1"/>
+    <col min="28" max="28" width="13" customWidth="1"/>
+    <col min="29" max="29" width="10.83203125" style="9"/>
+    <col min="30" max="30" width="13" customWidth="1"/>
+    <col min="31" max="31" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="25" customWidth="1"/>
+    <col min="35" max="35" width="24.33203125" customWidth="1"/>
+    <col min="36" max="36" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2080,42 +2083,44 @@
         <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AC1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>413</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
       <c r="AL1" s="1"/>
       <c r="AM1" s="1"/>
@@ -18461,8 +18466,9 @@
       <c r="XEY1" s="1"/>
       <c r="XEZ1" s="1"/>
       <c r="XFA1" s="1"/>
+      <c r="XFB1" s="1"/>
     </row>
-    <row r="2" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>205</v>
       </c>
@@ -18505,20 +18511,23 @@
       <c r="W2" t="s">
         <v>431</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="X2" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD2" t="s">
         <v>209</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>169</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>414</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="3" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>205</v>
       </c>
@@ -18561,17 +18570,20 @@
       <c r="W3" t="s">
         <v>431</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="X3" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD3" t="s">
         <v>210</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>169</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AI3" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="4" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>205</v>
       </c>
@@ -18614,20 +18626,23 @@
       <c r="W4" t="s">
         <v>431</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="X4" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD4" t="s">
         <v>211</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>169</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>414</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>205</v>
       </c>
@@ -18670,17 +18685,20 @@
       <c r="W5" t="s">
         <v>431</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="X5" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD5" t="s">
         <v>212</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>169</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="6" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>205</v>
       </c>
@@ -18723,17 +18741,20 @@
       <c r="W6" t="s">
         <v>431</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="X6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD6" t="s">
         <v>213</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>169</v>
       </c>
-      <c r="AH6" t="s">
+      <c r="AI6" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="7" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>205</v>
       </c>
@@ -18776,20 +18797,23 @@
       <c r="W7" t="s">
         <v>431</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="X7" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD7" t="s">
         <v>214</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>169</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AI7" t="s">
         <v>414</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AJ7" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="8" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>205</v>
       </c>
@@ -18832,17 +18856,20 @@
       <c r="W8" t="s">
         <v>431</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="X8" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD8" t="s">
         <v>215</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>169</v>
       </c>
-      <c r="AH8" t="s">
+      <c r="AI8" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="9" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>205</v>
       </c>
@@ -18885,17 +18912,20 @@
       <c r="W9" t="s">
         <v>431</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="X9" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD9" t="s">
         <v>216</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>169</v>
       </c>
-      <c r="AH9" t="s">
+      <c r="AI9" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="10" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>205</v>
       </c>
@@ -18938,20 +18968,23 @@
       <c r="W10" t="s">
         <v>431</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="X10" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD10" t="s">
         <v>217</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>169</v>
       </c>
-      <c r="AH10" t="s">
+      <c r="AI10" t="s">
         <v>414</v>
       </c>
-      <c r="AI10" t="s">
+      <c r="AJ10" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="11" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>205</v>
       </c>
@@ -18994,20 +19027,23 @@
       <c r="W11" t="s">
         <v>431</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="X11" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD11" t="s">
         <v>218</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>169</v>
       </c>
-      <c r="AH11" t="s">
+      <c r="AI11" t="s">
         <v>414</v>
       </c>
-      <c r="AI11" t="s">
+      <c r="AJ11" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="12" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>205</v>
       </c>
@@ -19050,17 +19086,20 @@
       <c r="W12" t="s">
         <v>431</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="X12" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD12" t="s">
         <v>219</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>169</v>
       </c>
-      <c r="AH12" t="s">
+      <c r="AI12" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>205</v>
       </c>
@@ -19103,20 +19142,23 @@
       <c r="W13" t="s">
         <v>431</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="X13" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD13" t="s">
         <v>220</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>169</v>
       </c>
-      <c r="AH13" t="s">
+      <c r="AI13" t="s">
         <v>414</v>
       </c>
-      <c r="AI13" t="s">
+      <c r="AJ13" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="14" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>205</v>
       </c>
@@ -19159,17 +19201,20 @@
       <c r="W14" t="s">
         <v>431</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="X14" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD14" t="s">
         <v>221</v>
       </c>
-      <c r="AD14" t="s">
+      <c r="AE14" t="s">
         <v>169</v>
       </c>
-      <c r="AH14" t="s">
+      <c r="AI14" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="15" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>205</v>
       </c>
@@ -19212,20 +19257,23 @@
       <c r="W15" t="s">
         <v>431</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="X15" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD15" t="s">
         <v>222</v>
       </c>
-      <c r="AD15" t="s">
+      <c r="AE15" t="s">
         <v>169</v>
       </c>
-      <c r="AH15" t="s">
+      <c r="AI15" t="s">
         <v>414</v>
       </c>
-      <c r="AI15" t="s">
+      <c r="AJ15" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="16" spans="1:16381" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16382" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>205</v>
       </c>
@@ -19268,17 +19316,20 @@
       <c r="W16" t="s">
         <v>431</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="X16" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD16" t="s">
         <v>223</v>
       </c>
-      <c r="AD16" t="s">
+      <c r="AE16" t="s">
         <v>169</v>
       </c>
-      <c r="AH16" t="s">
+      <c r="AI16" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>205</v>
       </c>
@@ -19321,20 +19372,23 @@
       <c r="W17" t="s">
         <v>431</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="X17" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD17" t="s">
         <v>224</v>
       </c>
-      <c r="AD17" t="s">
+      <c r="AE17" t="s">
         <v>169</v>
       </c>
-      <c r="AH17" t="s">
+      <c r="AI17" t="s">
         <v>414</v>
       </c>
-      <c r="AI17" t="s">
+      <c r="AJ17" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="18" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>205</v>
       </c>
@@ -19377,20 +19431,23 @@
       <c r="W18" t="s">
         <v>431</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="X18" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD18" t="s">
         <v>225</v>
       </c>
-      <c r="AD18" t="s">
+      <c r="AE18" t="s">
         <v>169</v>
       </c>
-      <c r="AH18" t="s">
+      <c r="AI18" t="s">
         <v>414</v>
       </c>
-      <c r="AI18" t="s">
+      <c r="AJ18" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="19" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>205</v>
       </c>
@@ -19433,20 +19490,23 @@
       <c r="W19" t="s">
         <v>431</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="X19" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD19" t="s">
         <v>226</v>
       </c>
-      <c r="AD19" t="s">
+      <c r="AE19" t="s">
         <v>169</v>
       </c>
-      <c r="AH19" t="s">
+      <c r="AI19" t="s">
         <v>414</v>
       </c>
-      <c r="AI19" t="s">
+      <c r="AJ19" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>205</v>
       </c>
@@ -19489,20 +19549,23 @@
       <c r="W20" t="s">
         <v>431</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="X20" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD20" t="s">
         <v>227</v>
       </c>
-      <c r="AD20" t="s">
+      <c r="AE20" t="s">
         <v>169</v>
       </c>
-      <c r="AH20" t="s">
+      <c r="AI20" t="s">
         <v>414</v>
       </c>
-      <c r="AI20" t="s">
+      <c r="AJ20" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>205</v>
       </c>
@@ -19545,20 +19608,23 @@
       <c r="W21" t="s">
         <v>431</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="X21" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD21" t="s">
         <v>228</v>
       </c>
-      <c r="AD21" t="s">
+      <c r="AE21" t="s">
         <v>169</v>
       </c>
-      <c r="AH21" t="s">
+      <c r="AI21" t="s">
         <v>414</v>
       </c>
-      <c r="AI21" t="s">
+      <c r="AJ21" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="22" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>205</v>
       </c>
@@ -19601,20 +19667,23 @@
       <c r="W22" t="s">
         <v>431</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="X22" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD22" t="s">
         <v>229</v>
       </c>
-      <c r="AD22" t="s">
+      <c r="AE22" t="s">
         <v>169</v>
       </c>
-      <c r="AH22" t="s">
+      <c r="AI22" t="s">
         <v>414</v>
       </c>
-      <c r="AI22" t="s">
+      <c r="AJ22" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>205</v>
       </c>
@@ -19657,20 +19726,23 @@
       <c r="W23" t="s">
         <v>431</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="X23" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD23" t="s">
         <v>230</v>
       </c>
-      <c r="AD23" t="s">
+      <c r="AE23" t="s">
         <v>169</v>
       </c>
-      <c r="AH23" t="s">
+      <c r="AI23" t="s">
         <v>414</v>
       </c>
-      <c r="AI23" t="s">
+      <c r="AJ23" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>205</v>
       </c>
@@ -19713,17 +19785,20 @@
       <c r="W24" t="s">
         <v>431</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="X24" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD24" t="s">
         <v>231</v>
       </c>
-      <c r="AD24" t="s">
+      <c r="AE24" t="s">
         <v>169</v>
       </c>
-      <c r="AH24" t="s">
+      <c r="AI24" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>205</v>
       </c>
@@ -19766,20 +19841,23 @@
       <c r="W25" t="s">
         <v>431</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="X25" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD25" t="s">
         <v>232</v>
       </c>
-      <c r="AD25" t="s">
+      <c r="AE25" t="s">
         <v>169</v>
       </c>
-      <c r="AH25" t="s">
+      <c r="AI25" t="s">
         <v>414</v>
       </c>
-      <c r="AI25" t="s">
+      <c r="AJ25" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>205</v>
       </c>
@@ -19822,20 +19900,23 @@
       <c r="W26" t="s">
         <v>431</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="X26" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD26" t="s">
         <v>233</v>
       </c>
-      <c r="AD26" t="s">
+      <c r="AE26" t="s">
         <v>169</v>
       </c>
-      <c r="AH26" t="s">
+      <c r="AI26" t="s">
         <v>414</v>
       </c>
-      <c r="AI26" t="s">
+      <c r="AJ26" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>205</v>
       </c>
@@ -19878,20 +19959,23 @@
       <c r="W27" t="s">
         <v>431</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="X27" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD27" t="s">
         <v>234</v>
       </c>
-      <c r="AD27" t="s">
+      <c r="AE27" t="s">
         <v>169</v>
       </c>
-      <c r="AH27" t="s">
+      <c r="AI27" t="s">
         <v>414</v>
       </c>
-      <c r="AI27" t="s">
+      <c r="AJ27" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>205</v>
       </c>
@@ -19934,20 +20018,23 @@
       <c r="W28" t="s">
         <v>431</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="X28" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD28" t="s">
         <v>235</v>
       </c>
-      <c r="AD28" t="s">
+      <c r="AE28" t="s">
         <v>169</v>
       </c>
-      <c r="AH28" t="s">
+      <c r="AI28" t="s">
         <v>414</v>
       </c>
-      <c r="AI28" t="s">
+      <c r="AJ28" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="29" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>205</v>
       </c>
@@ -19990,20 +20077,23 @@
       <c r="W29" t="s">
         <v>431</v>
       </c>
-      <c r="AC29" t="s">
+      <c r="X29" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD29" t="s">
         <v>236</v>
       </c>
-      <c r="AD29" t="s">
+      <c r="AE29" t="s">
         <v>169</v>
       </c>
-      <c r="AH29" t="s">
+      <c r="AI29" t="s">
         <v>414</v>
       </c>
-      <c r="AI29" t="s">
+      <c r="AJ29" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="30" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>205</v>
       </c>
@@ -20046,17 +20136,20 @@
       <c r="W30" t="s">
         <v>431</v>
       </c>
-      <c r="AC30" t="s">
+      <c r="X30" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD30" t="s">
         <v>237</v>
       </c>
-      <c r="AD30" t="s">
+      <c r="AE30" t="s">
         <v>169</v>
       </c>
-      <c r="AH30" t="s">
+      <c r="AI30" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>205</v>
       </c>
@@ -20099,20 +20192,23 @@
       <c r="W31" t="s">
         <v>431</v>
       </c>
-      <c r="AC31" t="s">
+      <c r="X31" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD31" t="s">
         <v>238</v>
       </c>
-      <c r="AD31" t="s">
+      <c r="AE31" t="s">
         <v>169</v>
       </c>
-      <c r="AH31" t="s">
+      <c r="AI31" t="s">
         <v>414</v>
       </c>
-      <c r="AI31" t="s">
+      <c r="AJ31" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>205</v>
       </c>
@@ -20149,11 +20245,14 @@
       <c r="W32" t="s">
         <v>431</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="X32" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA32" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="33" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>205</v>
       </c>
@@ -20196,20 +20295,23 @@
       <c r="W33" t="s">
         <v>431</v>
       </c>
-      <c r="AC33" t="s">
+      <c r="X33" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD33" t="s">
         <v>239</v>
       </c>
-      <c r="AD33" t="s">
+      <c r="AE33" t="s">
         <v>169</v>
       </c>
-      <c r="AH33" t="s">
+      <c r="AI33" t="s">
         <v>414</v>
       </c>
-      <c r="AI33" t="s">
+      <c r="AJ33" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="34" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>205</v>
       </c>
@@ -20252,20 +20354,23 @@
       <c r="W34" t="s">
         <v>431</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="X34" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD34" t="s">
         <v>240</v>
       </c>
-      <c r="AD34" t="s">
+      <c r="AE34" t="s">
         <v>169</v>
       </c>
-      <c r="AH34" t="s">
+      <c r="AI34" t="s">
         <v>414</v>
       </c>
-      <c r="AI34" t="s">
+      <c r="AJ34" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="35" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>205</v>
       </c>
@@ -20308,20 +20413,23 @@
       <c r="W35" t="s">
         <v>431</v>
       </c>
-      <c r="AC35" t="s">
+      <c r="X35" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD35" t="s">
         <v>241</v>
       </c>
-      <c r="AD35" t="s">
+      <c r="AE35" t="s">
         <v>169</v>
       </c>
-      <c r="AH35" t="s">
+      <c r="AI35" t="s">
         <v>414</v>
       </c>
-      <c r="AI35" t="s">
+      <c r="AJ35" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="36" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>205</v>
       </c>
@@ -20364,17 +20472,20 @@
       <c r="W36" t="s">
         <v>431</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="X36" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD36" t="s">
         <v>242</v>
       </c>
-      <c r="AD36" t="s">
+      <c r="AE36" t="s">
         <v>169</v>
       </c>
-      <c r="AH36" t="s">
+      <c r="AI36" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="37" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>205</v>
       </c>
@@ -20417,17 +20528,20 @@
       <c r="W37" t="s">
         <v>431</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="X37" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD37" t="s">
         <v>243</v>
       </c>
-      <c r="AD37" t="s">
+      <c r="AE37" t="s">
         <v>169</v>
       </c>
-      <c r="AH37" t="s">
+      <c r="AI37" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="38" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>205</v>
       </c>
@@ -20470,20 +20584,23 @@
       <c r="W38" t="s">
         <v>431</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="X38" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD38" t="s">
         <v>244</v>
       </c>
-      <c r="AD38" t="s">
+      <c r="AE38" t="s">
         <v>169</v>
       </c>
-      <c r="AH38" t="s">
+      <c r="AI38" t="s">
         <v>414</v>
       </c>
-      <c r="AI38" t="s">
+      <c r="AJ38" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="39" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>205</v>
       </c>
@@ -20526,17 +20643,20 @@
       <c r="W39" t="s">
         <v>431</v>
       </c>
-      <c r="AC39" t="s">
+      <c r="X39" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD39" t="s">
         <v>245</v>
       </c>
-      <c r="AD39" t="s">
+      <c r="AE39" t="s">
         <v>169</v>
       </c>
-      <c r="AH39" t="s">
+      <c r="AI39" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="40" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>205</v>
       </c>
@@ -20579,20 +20699,23 @@
       <c r="W40" t="s">
         <v>431</v>
       </c>
-      <c r="AC40" t="s">
+      <c r="X40" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD40" t="s">
         <v>246</v>
       </c>
-      <c r="AD40" t="s">
+      <c r="AE40" t="s">
         <v>169</v>
       </c>
-      <c r="AH40" t="s">
+      <c r="AI40" t="s">
         <v>414</v>
       </c>
-      <c r="AI40" t="s">
+      <c r="AJ40" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="41" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>205</v>
       </c>
@@ -20635,17 +20758,20 @@
       <c r="W41" t="s">
         <v>431</v>
       </c>
-      <c r="AC41" t="s">
+      <c r="X41" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD41" t="s">
         <v>247</v>
       </c>
-      <c r="AD41" t="s">
+      <c r="AE41" t="s">
         <v>169</v>
       </c>
-      <c r="AH41" t="s">
+      <c r="AI41" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="42" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>205</v>
       </c>
@@ -20688,17 +20814,20 @@
       <c r="W42" t="s">
         <v>431</v>
       </c>
-      <c r="AC42" t="s">
+      <c r="X42" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD42" t="s">
         <v>248</v>
       </c>
-      <c r="AD42" t="s">
+      <c r="AE42" t="s">
         <v>169</v>
       </c>
-      <c r="AH42" t="s">
+      <c r="AI42" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="43" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>205</v>
       </c>
@@ -20741,17 +20870,20 @@
       <c r="W43" t="s">
         <v>431</v>
       </c>
-      <c r="AC43" t="s">
+      <c r="X43" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD43" t="s">
         <v>249</v>
       </c>
-      <c r="AD43" t="s">
+      <c r="AE43" t="s">
         <v>169</v>
       </c>
-      <c r="AH43" t="s">
+      <c r="AI43" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="44" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>205</v>
       </c>
@@ -20794,17 +20926,20 @@
       <c r="W44" t="s">
         <v>431</v>
       </c>
-      <c r="AC44" t="s">
+      <c r="X44" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD44" t="s">
         <v>250</v>
       </c>
-      <c r="AD44" t="s">
+      <c r="AE44" t="s">
         <v>169</v>
       </c>
-      <c r="AH44" t="s">
+      <c r="AI44" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>205</v>
       </c>
@@ -20847,20 +20982,23 @@
       <c r="W45" t="s">
         <v>431</v>
       </c>
-      <c r="AC45" t="s">
+      <c r="X45" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD45" t="s">
         <v>251</v>
       </c>
-      <c r="AD45" t="s">
+      <c r="AE45" t="s">
         <v>169</v>
       </c>
-      <c r="AH45" t="s">
+      <c r="AI45" t="s">
         <v>414</v>
       </c>
-      <c r="AI45" t="s">
+      <c r="AJ45" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>205</v>
       </c>
@@ -20903,20 +21041,23 @@
       <c r="W46" t="s">
         <v>431</v>
       </c>
-      <c r="AC46" t="s">
+      <c r="X46" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD46" t="s">
         <v>252</v>
       </c>
-      <c r="AD46" t="s">
+      <c r="AE46" t="s">
         <v>169</v>
       </c>
-      <c r="AH46" t="s">
+      <c r="AI46" t="s">
         <v>414</v>
       </c>
-      <c r="AI46" t="s">
+      <c r="AJ46" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="47" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>205</v>
       </c>
@@ -20959,20 +21100,23 @@
       <c r="W47" t="s">
         <v>431</v>
       </c>
-      <c r="AC47" t="s">
+      <c r="X47" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD47" t="s">
         <v>253</v>
       </c>
-      <c r="AD47" t="s">
+      <c r="AE47" t="s">
         <v>169</v>
       </c>
-      <c r="AH47" t="s">
+      <c r="AI47" t="s">
         <v>414</v>
       </c>
-      <c r="AI47" t="s">
+      <c r="AJ47" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="48" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>205</v>
       </c>
@@ -21015,20 +21159,23 @@
       <c r="W48" t="s">
         <v>431</v>
       </c>
-      <c r="AC48" t="s">
+      <c r="X48" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD48" t="s">
         <v>254</v>
       </c>
-      <c r="AD48" t="s">
+      <c r="AE48" t="s">
         <v>169</v>
       </c>
-      <c r="AH48" t="s">
+      <c r="AI48" t="s">
         <v>414</v>
       </c>
-      <c r="AI48" t="s">
+      <c r="AJ48" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="49" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>205</v>
       </c>
@@ -21071,23 +21218,26 @@
       <c r="W49" t="s">
         <v>431</v>
       </c>
-      <c r="AC49" t="s">
+      <c r="X49" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD49" t="s">
         <v>255</v>
       </c>
-      <c r="AD49" t="s">
-        <v>170</v>
-      </c>
       <c r="AE49" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF49" t="s">
         <v>256</v>
       </c>
-      <c r="AH49" t="s">
+      <c r="AI49" t="s">
         <v>172</v>
       </c>
-      <c r="AI49" t="s">
+      <c r="AJ49" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="50" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>205</v>
       </c>
@@ -21133,20 +21283,23 @@
       <c r="W50" t="s">
         <v>431</v>
       </c>
-      <c r="AC50" t="s">
+      <c r="X50" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD50" t="s">
         <v>257</v>
       </c>
-      <c r="AD50" t="s">
-        <v>170</v>
-      </c>
       <c r="AE50" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF50" t="s">
         <v>258</v>
       </c>
-      <c r="AI50" t="s">
+      <c r="AJ50" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="51" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>205</v>
       </c>
@@ -21192,17 +21345,20 @@
       <c r="W51" t="s">
         <v>431</v>
       </c>
-      <c r="AC51" t="s">
+      <c r="X51" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD51" t="s">
         <v>259</v>
       </c>
-      <c r="AD51" t="s">
-        <v>170</v>
-      </c>
-      <c r="AI51" t="s">
+      <c r="AE51" t="s">
+        <v>170</v>
+      </c>
+      <c r="AJ51" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="52" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>205</v>
       </c>
@@ -21245,23 +21401,26 @@
       <c r="W52" t="s">
         <v>431</v>
       </c>
-      <c r="AC52" t="s">
+      <c r="X52" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD52" t="s">
         <v>260</v>
       </c>
-      <c r="AD52" t="s">
-        <v>170</v>
-      </c>
       <c r="AE52" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF52" t="s">
         <v>261</v>
       </c>
-      <c r="AH52" t="s">
+      <c r="AI52" t="s">
         <v>415</v>
       </c>
-      <c r="AI52" t="s">
+      <c r="AJ52" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="53" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>205</v>
       </c>
@@ -21304,23 +21463,26 @@
       <c r="W53" t="s">
         <v>431</v>
       </c>
-      <c r="AC53" t="s">
+      <c r="X53" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD53" t="s">
         <v>262</v>
       </c>
-      <c r="AD53" t="s">
-        <v>170</v>
-      </c>
       <c r="AE53" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF53" t="s">
         <v>263</v>
       </c>
-      <c r="AH53" t="s">
+      <c r="AI53" t="s">
         <v>415</v>
       </c>
-      <c r="AI53" t="s">
+      <c r="AJ53" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="54" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>205</v>
       </c>
@@ -21366,20 +21528,23 @@
       <c r="W54" t="s">
         <v>431</v>
       </c>
-      <c r="AC54" t="s">
+      <c r="X54" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD54" t="s">
         <v>264</v>
       </c>
-      <c r="AD54" t="s">
-        <v>170</v>
-      </c>
       <c r="AE54" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF54" t="s">
         <v>265</v>
       </c>
-      <c r="AI54" t="s">
+      <c r="AJ54" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>205</v>
       </c>
@@ -21422,23 +21587,26 @@
       <c r="W55" t="s">
         <v>431</v>
       </c>
-      <c r="AC55" t="s">
+      <c r="X55" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD55" t="s">
         <v>266</v>
       </c>
-      <c r="AD55" t="s">
-        <v>170</v>
-      </c>
       <c r="AE55" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF55" t="s">
         <v>267</v>
       </c>
-      <c r="AH55" t="s">
+      <c r="AI55" t="s">
         <v>416</v>
       </c>
-      <c r="AI55" t="s">
+      <c r="AJ55" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="56" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>205</v>
       </c>
@@ -21481,23 +21649,26 @@
       <c r="W56" t="s">
         <v>431</v>
       </c>
-      <c r="AC56" t="s">
+      <c r="X56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD56" t="s">
         <v>268</v>
       </c>
-      <c r="AD56" t="s">
-        <v>170</v>
-      </c>
       <c r="AE56" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF56" t="s">
         <v>269</v>
       </c>
-      <c r="AH56" t="s">
+      <c r="AI56" t="s">
         <v>416</v>
       </c>
-      <c r="AI56" t="s">
+      <c r="AJ56" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="57" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>205</v>
       </c>
@@ -21540,23 +21711,26 @@
       <c r="W57" t="s">
         <v>431</v>
       </c>
-      <c r="AC57" t="s">
+      <c r="X57" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD57" t="s">
         <v>270</v>
       </c>
-      <c r="AD57" t="s">
-        <v>170</v>
-      </c>
       <c r="AE57" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF57" t="s">
         <v>271</v>
       </c>
-      <c r="AH57" t="s">
+      <c r="AI57" t="s">
         <v>417</v>
       </c>
-      <c r="AI57" t="s">
+      <c r="AJ57" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="58" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
         <v>205</v>
       </c>
@@ -21602,23 +21776,26 @@
       <c r="W58" t="s">
         <v>431</v>
       </c>
-      <c r="AC58" t="s">
+      <c r="X58" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD58" t="s">
         <v>272</v>
       </c>
-      <c r="AD58" t="s">
-        <v>170</v>
-      </c>
       <c r="AE58" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF58" t="s">
         <v>273</v>
       </c>
-      <c r="AF58" t="s">
+      <c r="AG58" t="s">
         <v>274</v>
       </c>
-      <c r="AI58" t="s">
+      <c r="AJ58" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="59" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>205</v>
       </c>
@@ -21664,20 +21841,23 @@
       <c r="W59" t="s">
         <v>431</v>
       </c>
-      <c r="AC59" t="s">
+      <c r="X59" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD59" t="s">
         <v>275</v>
       </c>
-      <c r="AD59" t="s">
-        <v>170</v>
-      </c>
       <c r="AE59" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF59" t="s">
         <v>276</v>
       </c>
-      <c r="AI59" t="s">
+      <c r="AJ59" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="60" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>205</v>
       </c>
@@ -21720,23 +21900,26 @@
       <c r="W60" t="s">
         <v>431</v>
       </c>
-      <c r="AC60" t="s">
+      <c r="X60" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD60" t="s">
         <v>277</v>
       </c>
-      <c r="AD60" t="s">
-        <v>170</v>
-      </c>
       <c r="AE60" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF60" t="s">
         <v>278</v>
       </c>
-      <c r="AH60" t="s">
+      <c r="AI60" t="s">
         <v>418</v>
       </c>
-      <c r="AI60" t="s">
+      <c r="AJ60" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="61" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>205</v>
       </c>
@@ -21779,20 +21962,23 @@
       <c r="W61" t="s">
         <v>431</v>
       </c>
-      <c r="AC61" t="s">
+      <c r="X61" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD61" t="s">
         <v>279</v>
       </c>
-      <c r="AD61" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH61" t="s">
+      <c r="AE61" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI61" t="s">
         <v>175</v>
       </c>
-      <c r="AI61" t="s">
+      <c r="AJ61" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="62" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>205</v>
       </c>
@@ -21835,23 +22021,26 @@
       <c r="W62" t="s">
         <v>431</v>
       </c>
-      <c r="AC62" t="s">
+      <c r="X62" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD62" t="s">
         <v>280</v>
       </c>
-      <c r="AD62" t="s">
-        <v>170</v>
-      </c>
       <c r="AE62" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF62" t="s">
         <v>281</v>
       </c>
-      <c r="AH62" t="s">
+      <c r="AI62" t="s">
         <v>175</v>
       </c>
-      <c r="AI62" t="s">
+      <c r="AJ62" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>205</v>
       </c>
@@ -21894,20 +22083,23 @@
       <c r="W63" t="s">
         <v>431</v>
       </c>
-      <c r="AC63" t="s">
+      <c r="X63" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD63" t="s">
         <v>282</v>
       </c>
-      <c r="AD63" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH63" t="s">
+      <c r="AE63" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI63" t="s">
         <v>175</v>
       </c>
-      <c r="AI63" t="s">
+      <c r="AJ63" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="64" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>205</v>
       </c>
@@ -21953,20 +22145,23 @@
       <c r="W64" t="s">
         <v>431</v>
       </c>
-      <c r="AC64" t="s">
+      <c r="X64" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD64" t="s">
         <v>283</v>
       </c>
-      <c r="AD64" t="s">
-        <v>170</v>
-      </c>
       <c r="AE64" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF64" t="s">
         <v>284</v>
       </c>
-      <c r="AI64" t="s">
+      <c r="AJ64" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="65" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>205</v>
       </c>
@@ -22012,20 +22207,23 @@
       <c r="W65" t="s">
         <v>431</v>
       </c>
-      <c r="AC65" t="s">
+      <c r="X65" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD65" t="s">
         <v>283</v>
       </c>
-      <c r="AD65" t="s">
-        <v>170</v>
-      </c>
       <c r="AE65" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF65" t="s">
         <v>285</v>
       </c>
-      <c r="AI65" t="s">
+      <c r="AJ65" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="66" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>205</v>
       </c>
@@ -22071,20 +22269,23 @@
       <c r="W66" t="s">
         <v>431</v>
       </c>
-      <c r="AC66" t="s">
+      <c r="X66" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD66" t="s">
         <v>286</v>
       </c>
-      <c r="AD66" t="s">
-        <v>170</v>
-      </c>
       <c r="AE66" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF66" t="s">
         <v>287</v>
       </c>
-      <c r="AI66" t="s">
+      <c r="AJ66" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="67" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>205</v>
       </c>
@@ -22130,23 +22331,26 @@
       <c r="W67" t="s">
         <v>431</v>
       </c>
-      <c r="AC67" t="s">
+      <c r="X67" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD67" t="s">
         <v>288</v>
       </c>
-      <c r="AD67" t="s">
-        <v>170</v>
-      </c>
       <c r="AE67" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF67" t="s">
         <v>289</v>
       </c>
-      <c r="AH67" t="s">
+      <c r="AI67" t="s">
         <v>458</v>
       </c>
-      <c r="AI67" t="s">
+      <c r="AJ67" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="68" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>205</v>
       </c>
@@ -22192,23 +22396,26 @@
       <c r="W68" t="s">
         <v>431</v>
       </c>
-      <c r="AC68" t="s">
+      <c r="X68" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD68" t="s">
         <v>290</v>
       </c>
-      <c r="AD68" t="s">
-        <v>170</v>
-      </c>
       <c r="AE68" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF68" t="s">
         <v>291</v>
       </c>
-      <c r="AH68" t="s">
+      <c r="AI68" t="s">
         <v>458</v>
       </c>
-      <c r="AI68" t="s">
+      <c r="AJ68" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="69" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>205</v>
       </c>
@@ -22245,11 +22452,14 @@
       <c r="W69" t="s">
         <v>432</v>
       </c>
-      <c r="Z69" t="s">
+      <c r="X69" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA69" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="70" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>205</v>
       </c>
@@ -22286,11 +22496,14 @@
       <c r="W70" t="s">
         <v>432</v>
       </c>
-      <c r="Z70" t="s">
+      <c r="X70" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA70" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="71" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>205</v>
       </c>
@@ -22327,11 +22540,14 @@
       <c r="W71" t="s">
         <v>432</v>
       </c>
-      <c r="Z71" t="s">
+      <c r="X71" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA71" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="72" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>205</v>
       </c>
@@ -22368,11 +22584,14 @@
       <c r="W72" t="s">
         <v>432</v>
       </c>
-      <c r="Z72" t="s">
+      <c r="X72" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA72" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="73" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>205</v>
       </c>
@@ -22409,11 +22628,14 @@
       <c r="W73" t="s">
         <v>432</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="X73" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA73" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="74" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>205</v>
       </c>
@@ -22450,11 +22672,14 @@
       <c r="W74" t="s">
         <v>432</v>
       </c>
-      <c r="Z74" t="s">
+      <c r="X74" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA74" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="75" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>205</v>
       </c>
@@ -22500,23 +22725,26 @@
       <c r="W75" t="s">
         <v>431</v>
       </c>
-      <c r="AC75" t="s">
+      <c r="X75" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD75" t="s">
         <v>288</v>
       </c>
-      <c r="AD75" t="s">
-        <v>170</v>
-      </c>
       <c r="AE75" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF75" t="s">
         <v>292</v>
       </c>
-      <c r="AH75" t="s">
+      <c r="AI75" t="s">
         <v>458</v>
       </c>
-      <c r="AI75" t="s">
+      <c r="AJ75" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="76" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>205</v>
       </c>
@@ -22562,23 +22790,26 @@
       <c r="W76" t="s">
         <v>431</v>
       </c>
-      <c r="AC76" t="s">
+      <c r="X76" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD76" t="s">
         <v>288</v>
       </c>
-      <c r="AD76" t="s">
-        <v>170</v>
-      </c>
       <c r="AE76" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF76" t="s">
         <v>293</v>
       </c>
-      <c r="AH76" t="s">
+      <c r="AI76" t="s">
         <v>458</v>
       </c>
-      <c r="AI76" t="s">
+      <c r="AJ76" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="77" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>205</v>
       </c>
@@ -22622,26 +22853,29 @@
       <c r="W77" t="s">
         <v>431</v>
       </c>
-      <c r="AC77" t="s">
+      <c r="X77" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD77" t="s">
         <v>294</v>
       </c>
-      <c r="AD77" t="s">
-        <v>170</v>
-      </c>
       <c r="AE77" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF77" t="s">
         <v>295</v>
       </c>
-      <c r="AF77" t="s">
+      <c r="AG77" t="s">
         <v>296</v>
       </c>
-      <c r="AH77" t="s">
+      <c r="AI77" t="s">
         <v>178</v>
       </c>
-      <c r="AI77" t="s">
+      <c r="AJ77" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="78" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>205</v>
       </c>
@@ -22685,17 +22919,20 @@
       <c r="W78" t="s">
         <v>431</v>
       </c>
-      <c r="AC78" t="s">
+      <c r="X78" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD78" t="s">
         <v>297</v>
       </c>
-      <c r="AD78" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH78" t="s">
+      <c r="AE78" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI78" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="79" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>205</v>
       </c>
@@ -22739,26 +22976,29 @@
       <c r="W79" t="s">
         <v>431</v>
       </c>
-      <c r="AC79" t="s">
+      <c r="X79" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD79" t="s">
         <v>275</v>
       </c>
-      <c r="AD79" t="s">
-        <v>170</v>
-      </c>
       <c r="AE79" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF79" t="s">
         <v>298</v>
       </c>
-      <c r="AF79" t="s">
+      <c r="AG79" t="s">
         <v>299</v>
       </c>
-      <c r="AH79" t="s">
+      <c r="AI79" t="s">
         <v>179</v>
       </c>
-      <c r="AI79" t="s">
+      <c r="AJ79" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="80" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>205</v>
       </c>
@@ -22801,20 +23041,23 @@
       <c r="W80" t="s">
         <v>431</v>
       </c>
-      <c r="AC80" t="s">
+      <c r="X80" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD80" t="s">
         <v>300</v>
       </c>
-      <c r="AD80" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH80" t="s">
+      <c r="AE80" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI80" t="s">
         <v>179</v>
       </c>
-      <c r="AI80" t="s">
+      <c r="AJ80" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="81" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>205</v>
       </c>
@@ -22857,20 +23100,23 @@
       <c r="W81" t="s">
         <v>431</v>
       </c>
-      <c r="AC81" t="s">
+      <c r="X81" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD81" t="s">
         <v>301</v>
       </c>
-      <c r="AD81" t="s">
-        <v>170</v>
-      </c>
       <c r="AE81" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF81" t="s">
         <v>302</v>
       </c>
-      <c r="AH81" t="s">
+      <c r="AI81" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="82" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>205</v>
       </c>
@@ -22913,20 +23159,23 @@
       <c r="W82" t="s">
         <v>431</v>
       </c>
-      <c r="AC82" t="s">
+      <c r="X82" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD82" t="s">
         <v>303</v>
       </c>
-      <c r="AD82" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH82" t="s">
+      <c r="AE82" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI82" t="s">
         <v>181</v>
       </c>
-      <c r="AI82" t="s">
+      <c r="AJ82" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="83" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>205</v>
       </c>
@@ -22969,20 +23218,23 @@
       <c r="W83" t="s">
         <v>431</v>
       </c>
-      <c r="AC83" t="s">
+      <c r="X83" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD83" t="s">
         <v>304</v>
       </c>
-      <c r="AD83" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH83" t="s">
+      <c r="AE83" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI83" t="s">
         <v>181</v>
       </c>
-      <c r="AI83" t="s">
+      <c r="AJ83" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="84" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>205</v>
       </c>
@@ -23025,23 +23277,26 @@
       <c r="W84" t="s">
         <v>431</v>
       </c>
-      <c r="AC84" t="s">
+      <c r="X84" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD84" t="s">
         <v>305</v>
       </c>
-      <c r="AD84" t="s">
-        <v>170</v>
-      </c>
       <c r="AE84" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF84" t="s">
         <v>306</v>
       </c>
-      <c r="AH84" t="s">
+      <c r="AI84" t="s">
         <v>181</v>
       </c>
-      <c r="AI84" t="s">
+      <c r="AJ84" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="85" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>205</v>
       </c>
@@ -23084,17 +23339,20 @@
       <c r="W85" t="s">
         <v>431</v>
       </c>
-      <c r="AC85" t="s">
+      <c r="X85" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD85" t="s">
         <v>307</v>
       </c>
-      <c r="AD85" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH85" t="s">
+      <c r="AE85" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI85" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="86" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>205</v>
       </c>
@@ -23137,23 +23395,26 @@
       <c r="W86" t="s">
         <v>431</v>
       </c>
-      <c r="AC86" t="s">
+      <c r="X86" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD86" t="s">
         <v>308</v>
       </c>
-      <c r="AD86" t="s">
-        <v>170</v>
-      </c>
       <c r="AE86" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF86" t="s">
         <v>309</v>
       </c>
-      <c r="AH86" t="s">
+      <c r="AI86" t="s">
         <v>181</v>
       </c>
-      <c r="AI86" t="s">
+      <c r="AJ86" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="87" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>205</v>
       </c>
@@ -23196,23 +23457,26 @@
       <c r="W87" t="s">
         <v>431</v>
       </c>
-      <c r="AC87" t="s">
+      <c r="X87" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD87" t="s">
         <v>310</v>
       </c>
-      <c r="AD87" t="s">
-        <v>170</v>
-      </c>
       <c r="AE87" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF87" t="s">
         <v>311</v>
       </c>
-      <c r="AH87" t="s">
+      <c r="AI87" t="s">
         <v>181</v>
       </c>
-      <c r="AI87" t="s">
+      <c r="AJ87" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="88" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>205</v>
       </c>
@@ -23255,26 +23519,29 @@
       <c r="W88" t="s">
         <v>431</v>
       </c>
-      <c r="AC88" t="s">
+      <c r="X88" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD88" t="s">
         <v>312</v>
       </c>
-      <c r="AD88" t="s">
-        <v>170</v>
-      </c>
       <c r="AE88" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF88" t="s">
         <v>313</v>
       </c>
-      <c r="AF88" t="s">
+      <c r="AG88" t="s">
         <v>314</v>
       </c>
-      <c r="AH88" t="s">
+      <c r="AI88" t="s">
         <v>181</v>
       </c>
-      <c r="AI88" t="s">
+      <c r="AJ88" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="89" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>205</v>
       </c>
@@ -23317,23 +23584,26 @@
       <c r="W89" t="s">
         <v>431</v>
       </c>
-      <c r="AC89" t="s">
+      <c r="X89" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD89" t="s">
         <v>315</v>
       </c>
-      <c r="AD89" t="s">
-        <v>170</v>
-      </c>
       <c r="AE89" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF89" t="s">
         <v>316</v>
       </c>
-      <c r="AH89" t="s">
+      <c r="AI89" t="s">
         <v>181</v>
       </c>
-      <c r="AI89" t="s">
+      <c r="AJ89" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="90" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>205</v>
       </c>
@@ -23376,17 +23646,20 @@
       <c r="W90" t="s">
         <v>431</v>
       </c>
-      <c r="AC90" t="s">
+      <c r="X90" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD90" t="s">
         <v>317</v>
       </c>
-      <c r="AD90" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH90" t="s">
+      <c r="AE90" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI90" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="91" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>205</v>
       </c>
@@ -23429,23 +23702,26 @@
       <c r="W91" t="s">
         <v>431</v>
       </c>
-      <c r="AC91" t="s">
+      <c r="X91" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD91" t="s">
         <v>318</v>
       </c>
-      <c r="AD91" t="s">
-        <v>170</v>
-      </c>
       <c r="AE91" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF91" t="s">
         <v>319</v>
       </c>
-      <c r="AH91" t="s">
+      <c r="AI91" t="s">
         <v>181</v>
       </c>
-      <c r="AI91" t="s">
+      <c r="AJ91" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="92" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>205</v>
       </c>
@@ -23488,26 +23764,29 @@
       <c r="W92" t="s">
         <v>431</v>
       </c>
-      <c r="AC92" t="s">
+      <c r="X92" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD92" t="s">
         <v>320</v>
       </c>
-      <c r="AD92" t="s">
-        <v>170</v>
-      </c>
       <c r="AE92" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF92" t="s">
         <v>321</v>
       </c>
-      <c r="AF92" t="s">
+      <c r="AG92" t="s">
         <v>322</v>
       </c>
-      <c r="AH92" t="s">
+      <c r="AI92" t="s">
         <v>181</v>
       </c>
-      <c r="AI92" t="s">
+      <c r="AJ92" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="93" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>205</v>
       </c>
@@ -23550,20 +23829,23 @@
       <c r="W93" t="s">
         <v>431</v>
       </c>
-      <c r="AC93" t="s">
+      <c r="X93" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD93" t="s">
         <v>275</v>
       </c>
-      <c r="AD93" t="s">
-        <v>170</v>
-      </c>
       <c r="AE93" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF93" t="s">
         <v>323</v>
       </c>
-      <c r="AH93" t="s">
+      <c r="AI93" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>205</v>
       </c>
@@ -23606,23 +23888,26 @@
       <c r="W94" t="s">
         <v>431</v>
       </c>
-      <c r="AC94" t="s">
+      <c r="X94" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD94" t="s">
         <v>324</v>
       </c>
-      <c r="AD94" t="s">
-        <v>170</v>
-      </c>
       <c r="AE94" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF94" t="s">
         <v>319</v>
       </c>
-      <c r="AH94" t="s">
+      <c r="AI94" t="s">
         <v>181</v>
       </c>
-      <c r="AI94" t="s">
+      <c r="AJ94" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="95" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>205</v>
       </c>
@@ -23665,29 +23950,32 @@
       <c r="W95" t="s">
         <v>431</v>
       </c>
-      <c r="AC95" t="s">
+      <c r="X95" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD95" t="s">
         <v>325</v>
       </c>
-      <c r="AD95" t="s">
-        <v>170</v>
-      </c>
       <c r="AE95" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF95" t="s">
         <v>326</v>
       </c>
-      <c r="AF95" t="s">
+      <c r="AG95" t="s">
         <v>327</v>
       </c>
-      <c r="AG95" t="s">
+      <c r="AH95" t="s">
         <v>328</v>
       </c>
-      <c r="AH95" t="s">
+      <c r="AI95" t="s">
         <v>420</v>
       </c>
-      <c r="AI95" t="s">
+      <c r="AJ95" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="96" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>205</v>
       </c>
@@ -23724,11 +24012,14 @@
       <c r="W96" t="s">
         <v>432</v>
       </c>
-      <c r="Z96" t="s">
+      <c r="X96" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA96" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="97" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>205</v>
       </c>
@@ -23765,11 +24056,14 @@
       <c r="W97" t="s">
         <v>432</v>
       </c>
-      <c r="Z97" t="s">
+      <c r="X97" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA97" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="98" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>205</v>
       </c>
@@ -23812,20 +24106,23 @@
       <c r="W98" t="s">
         <v>431</v>
       </c>
-      <c r="AC98" t="s">
+      <c r="X98" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD98" t="s">
         <v>329</v>
       </c>
-      <c r="AD98" t="s">
-        <v>170</v>
-      </c>
       <c r="AE98" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF98" t="s">
         <v>330</v>
       </c>
-      <c r="AH98" t="s">
+      <c r="AI98" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="99" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>205</v>
       </c>
@@ -23868,20 +24165,23 @@
       <c r="W99" t="s">
         <v>431</v>
       </c>
-      <c r="AC99" t="s">
+      <c r="X99" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD99" t="s">
         <v>331</v>
       </c>
-      <c r="AD99" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH99" t="s">
+      <c r="AE99" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI99" t="s">
         <v>181</v>
       </c>
-      <c r="AI99" t="s">
+      <c r="AJ99" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="100" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>205</v>
       </c>
@@ -23924,23 +24224,26 @@
       <c r="W100" t="s">
         <v>431</v>
       </c>
-      <c r="AC100" t="s">
+      <c r="X100" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD100" t="s">
         <v>332</v>
       </c>
-      <c r="AD100" t="s">
-        <v>170</v>
-      </c>
       <c r="AE100" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF100" t="s">
         <v>333</v>
       </c>
-      <c r="AH100" t="s">
+      <c r="AI100" t="s">
         <v>184</v>
       </c>
-      <c r="AI100" t="s">
+      <c r="AJ100" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="101" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>205</v>
       </c>
@@ -23983,29 +24286,32 @@
       <c r="W101" t="s">
         <v>431</v>
       </c>
-      <c r="AC101" t="s">
+      <c r="X101" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD101" t="s">
         <v>330</v>
       </c>
-      <c r="AD101" t="s">
-        <v>170</v>
-      </c>
       <c r="AE101" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF101" t="s">
         <v>334</v>
       </c>
-      <c r="AF101" t="s">
+      <c r="AG101" t="s">
         <v>335</v>
       </c>
-      <c r="AG101" t="s">
+      <c r="AH101" t="s">
         <v>336</v>
       </c>
-      <c r="AH101" t="s">
+      <c r="AI101" t="s">
         <v>184</v>
       </c>
-      <c r="AI101" t="s">
+      <c r="AJ101" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="102" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>205</v>
       </c>
@@ -24048,26 +24354,29 @@
       <c r="W102" t="s">
         <v>431</v>
       </c>
-      <c r="AC102" t="s">
+      <c r="X102" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD102" t="s">
         <v>337</v>
       </c>
-      <c r="AD102" t="s">
-        <v>170</v>
-      </c>
       <c r="AE102" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF102" t="s">
         <v>338</v>
       </c>
-      <c r="AF102" t="s">
+      <c r="AG102" t="s">
         <v>339</v>
       </c>
-      <c r="AH102" t="s">
+      <c r="AI102" t="s">
         <v>184</v>
       </c>
-      <c r="AI102" t="s">
+      <c r="AJ102" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="103" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>205</v>
       </c>
@@ -24110,23 +24419,26 @@
       <c r="W103" t="s">
         <v>431</v>
       </c>
-      <c r="AC103" t="s">
+      <c r="X103" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD103" t="s">
         <v>340</v>
       </c>
-      <c r="AD103" t="s">
-        <v>170</v>
-      </c>
       <c r="AE103" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF103" t="s">
         <v>341</v>
       </c>
-      <c r="AH103" t="s">
+      <c r="AI103" t="s">
         <v>184</v>
       </c>
-      <c r="AI103" t="s">
+      <c r="AJ103" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="104" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>205</v>
       </c>
@@ -24169,23 +24481,26 @@
       <c r="W104" t="s">
         <v>431</v>
       </c>
-      <c r="AC104" t="s">
+      <c r="X104" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD104" t="s">
         <v>342</v>
       </c>
-      <c r="AD104" t="s">
-        <v>170</v>
-      </c>
       <c r="AE104" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF104" t="s">
         <v>343</v>
       </c>
-      <c r="AH104" t="s">
+      <c r="AI104" t="s">
         <v>184</v>
       </c>
-      <c r="AI104" t="s">
+      <c r="AJ104" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="105" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>205</v>
       </c>
@@ -24228,23 +24543,26 @@
       <c r="W105" t="s">
         <v>431</v>
       </c>
-      <c r="AC105" t="s">
+      <c r="X105" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD105" t="s">
         <v>340</v>
       </c>
-      <c r="AD105" t="s">
-        <v>170</v>
-      </c>
       <c r="AE105" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF105" t="s">
         <v>344</v>
       </c>
-      <c r="AH105" t="s">
+      <c r="AI105" t="s">
         <v>184</v>
       </c>
-      <c r="AI105" t="s">
+      <c r="AJ105" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="106" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>205</v>
       </c>
@@ -24281,11 +24599,14 @@
       <c r="W106" t="s">
         <v>432</v>
       </c>
-      <c r="Z106" t="s">
+      <c r="X106" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA106" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="107" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>205</v>
       </c>
@@ -24322,11 +24643,14 @@
       <c r="W107" t="s">
         <v>433</v>
       </c>
-      <c r="Z107" t="s">
+      <c r="X107" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA107" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="108" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>205</v>
       </c>
@@ -24363,11 +24687,14 @@
       <c r="W108" t="s">
         <v>433</v>
       </c>
-      <c r="Z108" t="s">
+      <c r="X108" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA108" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="109" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>205</v>
       </c>
@@ -24404,11 +24731,14 @@
       <c r="W109" t="s">
         <v>432</v>
       </c>
-      <c r="Z109" t="s">
+      <c r="X109" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA109" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="110" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>205</v>
       </c>
@@ -24445,11 +24775,14 @@
       <c r="W110" t="s">
         <v>433</v>
       </c>
-      <c r="Z110" t="s">
+      <c r="X110" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA110" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="111" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>205</v>
       </c>
@@ -24486,11 +24819,14 @@
       <c r="W111" t="s">
         <v>433</v>
       </c>
-      <c r="Z111" t="s">
+      <c r="X111" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA111" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="112" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>205</v>
       </c>
@@ -24533,23 +24869,26 @@
       <c r="W112" t="s">
         <v>431</v>
       </c>
-      <c r="AD112" t="s">
+      <c r="X112" t="s">
         <v>170</v>
       </c>
       <c r="AE112" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF112" t="s">
         <v>345</v>
       </c>
-      <c r="AF112" t="s">
+      <c r="AG112" t="s">
         <v>346</v>
       </c>
-      <c r="AH112" t="s">
+      <c r="AI112" t="s">
         <v>184</v>
       </c>
-      <c r="AI112" t="s">
+      <c r="AJ112" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="113" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>205</v>
       </c>
@@ -24592,23 +24931,26 @@
       <c r="W113" t="s">
         <v>431</v>
       </c>
-      <c r="AC113" t="s">
+      <c r="X113" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD113" t="s">
         <v>347</v>
       </c>
-      <c r="AD113" t="s">
-        <v>170</v>
-      </c>
       <c r="AE113" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF113" t="s">
         <v>348</v>
       </c>
-      <c r="AH113" t="s">
+      <c r="AI113" t="s">
         <v>185</v>
       </c>
-      <c r="AI113" t="s">
+      <c r="AJ113" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="114" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>205</v>
       </c>
@@ -24651,20 +24993,23 @@
       <c r="W114" t="s">
         <v>431</v>
       </c>
-      <c r="AC114" t="s">
+      <c r="X114" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD114" t="s">
         <v>349</v>
       </c>
-      <c r="AD114" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH114" t="s">
+      <c r="AE114" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI114" t="s">
         <v>185</v>
       </c>
-      <c r="AI114" t="s">
+      <c r="AJ114" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="115" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>205</v>
       </c>
@@ -24707,20 +25052,23 @@
       <c r="W115" t="s">
         <v>431</v>
       </c>
-      <c r="AC115" t="s">
+      <c r="X115" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD115" t="s">
         <v>350</v>
       </c>
-      <c r="AD115" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH115" t="s">
+      <c r="AE115" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI115" t="s">
         <v>185</v>
       </c>
-      <c r="AI115" t="s">
+      <c r="AJ115" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="116" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>205</v>
       </c>
@@ -24763,17 +25111,20 @@
       <c r="W116" t="s">
         <v>431</v>
       </c>
-      <c r="AC116" t="s">
+      <c r="X116" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD116" t="s">
         <v>351</v>
       </c>
-      <c r="AH116" t="s">
+      <c r="AI116" t="s">
         <v>185</v>
       </c>
-      <c r="AI116" t="s">
+      <c r="AJ116" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>205</v>
       </c>
@@ -24816,17 +25167,20 @@
       <c r="W117" t="s">
         <v>431</v>
       </c>
-      <c r="AC117" t="s">
+      <c r="X117" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD117" t="s">
         <v>352</v>
       </c>
-      <c r="AH117" t="s">
+      <c r="AI117" t="s">
         <v>185</v>
       </c>
-      <c r="AI117" t="s">
+      <c r="AJ117" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="118" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>205</v>
       </c>
@@ -24869,26 +25223,29 @@
       <c r="W118" t="s">
         <v>431</v>
       </c>
-      <c r="AC118" t="s">
+      <c r="X118" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD118" t="s">
         <v>353</v>
       </c>
-      <c r="AD118" t="s">
-        <v>170</v>
-      </c>
       <c r="AE118" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF118" t="s">
         <v>354</v>
       </c>
-      <c r="AF118" t="s">
+      <c r="AG118" t="s">
         <v>355</v>
       </c>
-      <c r="AH118" t="s">
+      <c r="AI118" t="s">
         <v>421</v>
       </c>
-      <c r="AI118" t="s">
+      <c r="AJ118" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="119" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>205</v>
       </c>
@@ -24931,26 +25288,29 @@
       <c r="W119" t="s">
         <v>431</v>
       </c>
-      <c r="AC119" t="s">
+      <c r="X119" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD119" t="s">
         <v>356</v>
       </c>
-      <c r="AD119" t="s">
-        <v>170</v>
-      </c>
       <c r="AE119" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF119" t="s">
         <v>357</v>
       </c>
-      <c r="AF119" t="s">
+      <c r="AG119" t="s">
         <v>358</v>
       </c>
-      <c r="AH119" t="s">
+      <c r="AI119" t="s">
         <v>422</v>
       </c>
-      <c r="AI119" t="s">
+      <c r="AJ119" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="120" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>205</v>
       </c>
@@ -24987,11 +25347,14 @@
       <c r="W120" t="s">
         <v>432</v>
       </c>
-      <c r="Z120" t="s">
+      <c r="X120" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA120" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="121" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>205</v>
       </c>
@@ -25028,11 +25391,14 @@
       <c r="W121" t="s">
         <v>432</v>
       </c>
-      <c r="Z121" t="s">
+      <c r="X121" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA121" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="122" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>205</v>
       </c>
@@ -25069,11 +25435,14 @@
       <c r="W122" t="s">
         <v>432</v>
       </c>
-      <c r="Z122" t="s">
+      <c r="X122" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA122" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="123" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>205</v>
       </c>
@@ -25110,11 +25479,14 @@
       <c r="W123" t="s">
         <v>432</v>
       </c>
-      <c r="Z123" t="s">
+      <c r="X123" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA123" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="124" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>205</v>
       </c>
@@ -25157,23 +25529,26 @@
       <c r="W124" t="s">
         <v>431</v>
       </c>
-      <c r="AC124" t="s">
+      <c r="X124" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD124" t="s">
         <v>330</v>
       </c>
-      <c r="AD124" t="s">
-        <v>170</v>
-      </c>
       <c r="AE124" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF124" t="s">
         <v>359</v>
       </c>
-      <c r="AH124" t="s">
+      <c r="AI124" t="s">
         <v>185</v>
       </c>
-      <c r="AI124" t="s">
+      <c r="AJ124" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="125" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>205</v>
       </c>
@@ -25216,23 +25591,26 @@
       <c r="W125" t="s">
         <v>431</v>
       </c>
-      <c r="AC125" t="s">
+      <c r="X125" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD125" t="s">
         <v>360</v>
       </c>
-      <c r="AD125" t="s">
-        <v>170</v>
-      </c>
       <c r="AE125" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF125" t="s">
         <v>361</v>
       </c>
-      <c r="AH125" t="s">
+      <c r="AI125" t="s">
         <v>422</v>
       </c>
-      <c r="AI125" t="s">
+      <c r="AJ125" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="126" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>205</v>
       </c>
@@ -25275,23 +25653,26 @@
       <c r="W126" t="s">
         <v>431</v>
       </c>
-      <c r="AC126" t="s">
+      <c r="X126" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD126" t="s">
         <v>362</v>
       </c>
-      <c r="AD126" t="s">
-        <v>170</v>
-      </c>
       <c r="AE126" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF126" t="s">
         <v>363</v>
       </c>
-      <c r="AH126" t="s">
+      <c r="AI126" t="s">
         <v>185</v>
       </c>
-      <c r="AI126" t="s">
+      <c r="AJ126" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="127" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>205</v>
       </c>
@@ -25334,23 +25715,26 @@
       <c r="W127" t="s">
         <v>431</v>
       </c>
-      <c r="AC127" t="s">
+      <c r="X127" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD127" t="s">
         <v>362</v>
       </c>
-      <c r="AD127" t="s">
-        <v>170</v>
-      </c>
       <c r="AE127" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF127" t="s">
         <v>364</v>
       </c>
-      <c r="AH127" t="s">
+      <c r="AI127" t="s">
         <v>423</v>
       </c>
-      <c r="AI127" t="s">
+      <c r="AJ127" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="128" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>205</v>
       </c>
@@ -25393,23 +25777,26 @@
       <c r="W128" t="s">
         <v>431</v>
       </c>
-      <c r="AC128" t="s">
+      <c r="X128" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD128" t="s">
         <v>347</v>
       </c>
-      <c r="AD128" t="s">
-        <v>170</v>
-      </c>
       <c r="AE128" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF128" t="s">
         <v>365</v>
       </c>
-      <c r="AH128" t="s">
+      <c r="AI128" t="s">
         <v>424</v>
       </c>
-      <c r="AI128" t="s">
+      <c r="AJ128" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="129" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>205</v>
       </c>
@@ -25452,29 +25839,32 @@
       <c r="W129" t="s">
         <v>431</v>
       </c>
-      <c r="AC129" t="s">
+      <c r="X129" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD129" t="s">
         <v>319</v>
       </c>
-      <c r="AD129" t="s">
-        <v>170</v>
-      </c>
       <c r="AE129" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF129" t="s">
         <v>366</v>
       </c>
-      <c r="AF129" t="s">
+      <c r="AG129" t="s">
         <v>367</v>
       </c>
-      <c r="AG129" t="s">
+      <c r="AH129" t="s">
         <v>368</v>
       </c>
-      <c r="AH129" s="10" t="s">
+      <c r="AI129" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="AI129" t="s">
+      <c r="AJ129" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="130" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>205</v>
       </c>
@@ -25517,23 +25907,26 @@
       <c r="W130" t="s">
         <v>431</v>
       </c>
-      <c r="AC130" t="s">
+      <c r="X130" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD130" t="s">
         <v>319</v>
       </c>
-      <c r="AD130" t="s">
-        <v>170</v>
-      </c>
       <c r="AE130" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF130" t="s">
         <v>369</v>
       </c>
-      <c r="AH130" s="11" t="s">
+      <c r="AI130" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="AI130" t="s">
+      <c r="AJ130" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="131" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>205</v>
       </c>
@@ -25576,23 +25969,26 @@
       <c r="W131" t="s">
         <v>431</v>
       </c>
-      <c r="AC131" t="s">
+      <c r="X131" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD131" t="s">
         <v>319</v>
       </c>
-      <c r="AD131" t="s">
-        <v>170</v>
-      </c>
       <c r="AE131" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF131" t="s">
         <v>370</v>
       </c>
-      <c r="AH131" t="s">
+      <c r="AI131" t="s">
         <v>185</v>
       </c>
-      <c r="AI131" t="s">
+      <c r="AJ131" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="132" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>205</v>
       </c>
@@ -25635,20 +26031,23 @@
       <c r="W132" t="s">
         <v>431</v>
       </c>
-      <c r="AC132" t="s">
+      <c r="X132" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD132" t="s">
         <v>371</v>
       </c>
-      <c r="AD132" t="s">
-        <v>170</v>
-      </c>
       <c r="AE132" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF132" t="s">
         <v>275</v>
       </c>
-      <c r="AH132" t="s">
+      <c r="AI132" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="133" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>205</v>
       </c>
@@ -25691,20 +26090,23 @@
       <c r="W133" t="s">
         <v>431</v>
       </c>
-      <c r="AC133" t="s">
+      <c r="X133" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD133" t="s">
         <v>372</v>
       </c>
-      <c r="AD133" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH133" t="s">
+      <c r="AE133" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI133" t="s">
         <v>185</v>
       </c>
-      <c r="AI133" t="s">
+      <c r="AJ133" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="134" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>205</v>
       </c>
@@ -25747,20 +26149,23 @@
       <c r="W134" t="s">
         <v>431</v>
       </c>
-      <c r="AC134" t="s">
+      <c r="X134" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD134" t="s">
         <v>373</v>
       </c>
-      <c r="AD134" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH134" t="s">
+      <c r="AE134" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI134" t="s">
         <v>185</v>
       </c>
-      <c r="AI134" t="s">
+      <c r="AJ134" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>205</v>
       </c>
@@ -25803,20 +26208,23 @@
       <c r="W135" t="s">
         <v>431</v>
       </c>
-      <c r="AC135" t="s">
+      <c r="X135" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD135" t="s">
         <v>374</v>
       </c>
-      <c r="AD135" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH135" t="s">
+      <c r="AE135" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI135" t="s">
         <v>185</v>
       </c>
-      <c r="AI135" t="s">
+      <c r="AJ135" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="136" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>205</v>
       </c>
@@ -25859,20 +26267,23 @@
       <c r="W136" t="s">
         <v>431</v>
       </c>
-      <c r="AC136" t="s">
+      <c r="X136" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD136" t="s">
         <v>375</v>
       </c>
-      <c r="AD136" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH136" t="s">
+      <c r="AE136" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI136" t="s">
         <v>185</v>
       </c>
-      <c r="AI136" t="s">
+      <c r="AJ136" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="137" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>205</v>
       </c>
@@ -25915,20 +26326,23 @@
       <c r="W137" t="s">
         <v>431</v>
       </c>
-      <c r="AC137" t="s">
+      <c r="X137" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD137" t="s">
         <v>376</v>
       </c>
-      <c r="AD137" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH137" t="s">
+      <c r="AE137" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI137" t="s">
         <v>185</v>
       </c>
-      <c r="AI137" t="s">
+      <c r="AJ137" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="138" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>205</v>
       </c>
@@ -25971,20 +26385,23 @@
       <c r="W138" t="s">
         <v>431</v>
       </c>
-      <c r="AC138" t="s">
+      <c r="X138" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD138" t="s">
         <v>377</v>
       </c>
-      <c r="AD138" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH138" t="s">
+      <c r="AE138" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI138" t="s">
         <v>185</v>
       </c>
-      <c r="AI138" t="s">
+      <c r="AJ138" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="139" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>205</v>
       </c>
@@ -26027,20 +26444,23 @@
       <c r="W139" t="s">
         <v>431</v>
       </c>
-      <c r="AC139" t="s">
+      <c r="X139" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD139" t="s">
         <v>378</v>
       </c>
-      <c r="AD139" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH139" t="s">
+      <c r="AE139" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI139" t="s">
         <v>185</v>
       </c>
-      <c r="AI139" t="s">
+      <c r="AJ139" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="140" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>205</v>
       </c>
@@ -26083,20 +26503,23 @@
       <c r="W140" t="s">
         <v>431</v>
       </c>
-      <c r="AC140" t="s">
+      <c r="X140" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD140" t="s">
         <v>379</v>
       </c>
-      <c r="AD140" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH140" t="s">
+      <c r="AE140" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI140" t="s">
         <v>190</v>
       </c>
-      <c r="AI140" t="s">
+      <c r="AJ140" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="141" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>205</v>
       </c>
@@ -26139,17 +26562,20 @@
       <c r="W141" t="s">
         <v>431</v>
       </c>
-      <c r="AC141" t="s">
+      <c r="X141" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD141" t="s">
         <v>332</v>
       </c>
-      <c r="AD141" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH141" t="s">
+      <c r="AE141" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI141" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="142" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>205</v>
       </c>
@@ -26192,20 +26618,23 @@
       <c r="W142" t="s">
         <v>431</v>
       </c>
-      <c r="AC142" t="s">
+      <c r="X142" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD142" t="s">
         <v>380</v>
       </c>
-      <c r="AD142" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH142" t="s">
+      <c r="AE142" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI142" t="s">
         <v>190</v>
       </c>
-      <c r="AI142" t="s">
+      <c r="AJ142" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="143" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>205</v>
       </c>
@@ -26248,17 +26677,20 @@
       <c r="W143" t="s">
         <v>431</v>
       </c>
-      <c r="AC143" t="s">
+      <c r="X143" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD143" t="s">
         <v>381</v>
       </c>
-      <c r="AD143" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH143" t="s">
+      <c r="AE143" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI143" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="144" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>205</v>
       </c>
@@ -26301,17 +26733,20 @@
       <c r="W144" t="s">
         <v>431</v>
       </c>
-      <c r="AC144" t="s">
+      <c r="X144" t="s">
+        <v>170</v>
+      </c>
+      <c r="AD144" t="s">
         <v>332</v>
       </c>
-      <c r="AD144" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH144" t="s">
+      <c r="AE144" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI144" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="145" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>205</v>
       </c>
@@ -26357,14 +26792,17 @@
       <c r="W145" t="s">
         <v>431</v>
       </c>
-      <c r="AD145" t="s">
-        <v>170</v>
-      </c>
-      <c r="AH145" t="s">
+      <c r="X145" t="s">
+        <v>170</v>
+      </c>
+      <c r="AE145" t="s">
+        <v>170</v>
+      </c>
+      <c r="AI145" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="146" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>205</v>
       </c>
@@ -26410,11 +26848,14 @@
       <c r="W146" t="s">
         <v>431</v>
       </c>
-      <c r="Z146" t="s">
+      <c r="X146" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA146" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="147" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>205</v>
       </c>
@@ -26460,23 +26901,26 @@
       <c r="W147" t="s">
         <v>432</v>
       </c>
-      <c r="Z147" t="s">
+      <c r="X147" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA147" t="s">
         <v>506</v>
       </c>
-      <c r="AC147" t="s">
+      <c r="AD147" t="s">
         <v>382</v>
       </c>
-      <c r="AD147" t="s">
-        <v>170</v>
-      </c>
       <c r="AE147" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF147" t="s">
         <v>383</v>
       </c>
-      <c r="AF147" t="s">
+      <c r="AG147" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="148" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>205</v>
       </c>
@@ -26516,23 +26960,26 @@
       <c r="W148" t="s">
         <v>432</v>
       </c>
-      <c r="Z148" t="s">
+      <c r="X148" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA148" t="s">
         <v>506</v>
       </c>
-      <c r="AC148" t="s">
+      <c r="AD148" t="s">
         <v>382</v>
       </c>
-      <c r="AD148" t="s">
-        <v>170</v>
-      </c>
       <c r="AE148" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF148" t="s">
         <v>385</v>
       </c>
-      <c r="AF148" t="s">
+      <c r="AG148" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="149" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B149" t="s">
         <v>205</v>
       </c>
@@ -26572,23 +27019,26 @@
       <c r="W149" t="s">
         <v>432</v>
       </c>
-      <c r="Z149" t="s">
+      <c r="X149" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA149" t="s">
         <v>506</v>
       </c>
-      <c r="AC149" t="s">
+      <c r="AD149" t="s">
         <v>382</v>
       </c>
-      <c r="AD149" t="s">
-        <v>170</v>
-      </c>
       <c r="AE149" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF149" t="s">
         <v>386</v>
       </c>
-      <c r="AF149" t="s">
+      <c r="AG149" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="150" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B150" t="s">
         <v>205</v>
       </c>
@@ -26628,26 +27078,29 @@
       <c r="W150" t="s">
         <v>432</v>
       </c>
-      <c r="Z150" t="s">
+      <c r="X150" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA150" t="s">
         <v>506</v>
       </c>
-      <c r="AC150" t="s">
+      <c r="AD150" t="s">
         <v>382</v>
       </c>
-      <c r="AD150" t="s">
-        <v>170</v>
-      </c>
       <c r="AE150" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF150" t="s">
         <v>387</v>
       </c>
-      <c r="AF150" t="s">
+      <c r="AG150" t="s">
         <v>319</v>
       </c>
-      <c r="AI150" t="s">
+      <c r="AJ150" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="151" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>205</v>
       </c>
@@ -26684,26 +27137,29 @@
       <c r="W151" t="s">
         <v>432</v>
       </c>
-      <c r="Z151" t="s">
+      <c r="X151" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA151" t="s">
         <v>506</v>
       </c>
-      <c r="AC151" t="s">
+      <c r="AD151" t="s">
         <v>382</v>
       </c>
-      <c r="AD151" t="s">
-        <v>170</v>
-      </c>
       <c r="AE151" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF151" t="s">
         <v>388</v>
       </c>
-      <c r="AF151" t="s">
+      <c r="AG151" t="s">
         <v>384</v>
       </c>
-      <c r="AG151" t="s">
+      <c r="AH151" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="152" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B152" t="s">
         <v>205</v>
       </c>
@@ -26743,11 +27199,14 @@
       <c r="W152" t="s">
         <v>431</v>
       </c>
-      <c r="Z152" t="s">
+      <c r="X152" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA152" t="s">
         <v>506</v>
       </c>
     </row>
-    <row r="153" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>205</v>
       </c>
@@ -26787,23 +27246,26 @@
       <c r="W153" t="s">
         <v>432</v>
       </c>
-      <c r="Z153" t="s">
+      <c r="X153" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA153" t="s">
         <v>506</v>
       </c>
-      <c r="AC153" t="s">
+      <c r="AD153" t="s">
         <v>390</v>
       </c>
-      <c r="AD153" t="s">
-        <v>170</v>
-      </c>
       <c r="AE153" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF153" t="s">
         <v>391</v>
       </c>
-      <c r="AI153" t="s">
+      <c r="AJ153" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="154" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B154" t="s">
         <v>205</v>
       </c>
@@ -26843,23 +27305,26 @@
       <c r="W154" t="s">
         <v>432</v>
       </c>
-      <c r="Z154" t="s">
+      <c r="X154" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA154" t="s">
         <v>506</v>
       </c>
-      <c r="AC154" t="s">
+      <c r="AD154" t="s">
         <v>392</v>
       </c>
-      <c r="AD154" t="s">
-        <v>170</v>
-      </c>
       <c r="AE154" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF154" t="s">
         <v>393</v>
       </c>
-      <c r="AI154" t="s">
+      <c r="AJ154" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="155" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>205</v>
       </c>
@@ -26899,23 +27364,26 @@
       <c r="W155" t="s">
         <v>432</v>
       </c>
-      <c r="Z155" t="s">
+      <c r="X155" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA155" t="s">
         <v>506</v>
       </c>
-      <c r="AC155" t="s">
+      <c r="AD155" t="s">
         <v>394</v>
       </c>
-      <c r="AD155" t="s">
-        <v>170</v>
-      </c>
       <c r="AE155" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF155" t="s">
         <v>395</v>
       </c>
-      <c r="AI155" t="s">
+      <c r="AJ155" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="156" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>205</v>
       </c>
@@ -26955,23 +27423,26 @@
       <c r="W156" t="s">
         <v>432</v>
       </c>
-      <c r="Z156" t="s">
+      <c r="X156" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA156" t="s">
         <v>506</v>
       </c>
-      <c r="AC156" t="s">
+      <c r="AD156" t="s">
         <v>396</v>
       </c>
-      <c r="AD156" t="s">
-        <v>170</v>
-      </c>
       <c r="AE156" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF156" t="s">
         <v>397</v>
       </c>
-      <c r="AI156" t="s">
+      <c r="AJ156" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="157" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>205</v>
       </c>
@@ -27011,23 +27482,26 @@
       <c r="W157" t="s">
         <v>432</v>
       </c>
-      <c r="Z157" t="s">
+      <c r="X157" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA157" t="s">
         <v>506</v>
       </c>
-      <c r="AC157" t="s">
+      <c r="AD157" t="s">
         <v>398</v>
       </c>
-      <c r="AD157" t="s">
-        <v>170</v>
-      </c>
       <c r="AE157" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF157" t="s">
         <v>399</v>
       </c>
-      <c r="AI157" t="s">
+      <c r="AJ157" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="158" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>205</v>
       </c>
@@ -27067,23 +27541,26 @@
       <c r="W158" t="s">
         <v>432</v>
       </c>
-      <c r="Z158" t="s">
+      <c r="X158" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA158" t="s">
         <v>506</v>
       </c>
-      <c r="AC158" t="s">
+      <c r="AD158" t="s">
         <v>400</v>
       </c>
-      <c r="AD158" t="s">
-        <v>170</v>
-      </c>
       <c r="AE158" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF158" t="s">
         <v>401</v>
       </c>
-      <c r="AI158" t="s">
+      <c r="AJ158" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="159" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>205</v>
       </c>
@@ -27123,23 +27600,26 @@
       <c r="W159" t="s">
         <v>432</v>
       </c>
-      <c r="Z159" t="s">
+      <c r="X159" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA159" t="s">
         <v>506</v>
       </c>
-      <c r="AC159" t="s">
+      <c r="AD159" t="s">
         <v>402</v>
       </c>
-      <c r="AD159" t="s">
-        <v>170</v>
-      </c>
       <c r="AE159" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF159" t="s">
         <v>403</v>
       </c>
-      <c r="AI159" t="s">
+      <c r="AJ159" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="160" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>205</v>
       </c>
@@ -27179,23 +27659,26 @@
       <c r="W160" t="s">
         <v>432</v>
       </c>
-      <c r="Z160" t="s">
+      <c r="X160" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA160" t="s">
         <v>506</v>
       </c>
-      <c r="AC160" t="s">
+      <c r="AD160" t="s">
         <v>404</v>
       </c>
-      <c r="AD160" t="s">
-        <v>170</v>
-      </c>
       <c r="AE160" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF160" t="s">
         <v>405</v>
       </c>
-      <c r="AI160" t="s">
+      <c r="AJ160" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="161" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B161" t="s">
         <v>205</v>
       </c>
@@ -27235,23 +27718,26 @@
       <c r="W161" t="s">
         <v>432</v>
       </c>
-      <c r="Z161" t="s">
+      <c r="X161" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA161" t="s">
         <v>506</v>
       </c>
-      <c r="AC161" t="s">
+      <c r="AD161" t="s">
         <v>406</v>
       </c>
-      <c r="AD161" t="s">
-        <v>170</v>
-      </c>
       <c r="AE161" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF161" t="s">
         <v>407</v>
       </c>
-      <c r="AI161" t="s">
+      <c r="AJ161" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="162" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B162" t="s">
         <v>205</v>
       </c>
@@ -27291,23 +27777,26 @@
       <c r="W162" t="s">
         <v>432</v>
       </c>
-      <c r="Z162" t="s">
+      <c r="X162" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA162" t="s">
         <v>506</v>
       </c>
-      <c r="AC162" t="s">
+      <c r="AD162" t="s">
         <v>408</v>
       </c>
-      <c r="AD162" t="s">
-        <v>170</v>
-      </c>
       <c r="AE162" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF162" t="s">
         <v>409</v>
       </c>
-      <c r="AI162" t="s">
+      <c r="AJ162" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="163" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B163" t="s">
         <v>205</v>
       </c>
@@ -27347,23 +27836,26 @@
       <c r="W163" t="s">
         <v>432</v>
       </c>
-      <c r="Z163" t="s">
+      <c r="X163" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA163" t="s">
         <v>506</v>
       </c>
-      <c r="AC163" t="s">
+      <c r="AD163" t="s">
         <v>410</v>
       </c>
-      <c r="AD163" t="s">
-        <v>170</v>
-      </c>
       <c r="AE163" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF163" t="s">
         <v>411</v>
       </c>
-      <c r="AI163" t="s">
+      <c r="AJ163" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="164" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B164" t="s">
         <v>205</v>
       </c>
@@ -27400,39 +27892,42 @@
       <c r="W164" t="s">
         <v>432</v>
       </c>
-      <c r="Z164" t="s">
+      <c r="X164" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA164" t="s">
         <v>506</v>
       </c>
-      <c r="AC164" t="s">
+      <c r="AD164" t="s">
         <v>503</v>
       </c>
-      <c r="AD164" t="s">
-        <v>170</v>
-      </c>
       <c r="AE164" t="s">
+        <v>170</v>
+      </c>
+      <c r="AF164" t="s">
         <v>412</v>
       </c>
-      <c r="AI164" t="s">
+      <c r="AJ164" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="165" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:36" x14ac:dyDescent="0.2">
       <c r="N165" s="7"/>
       <c r="O165" s="7"/>
     </row>
-    <row r="166" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:36" x14ac:dyDescent="0.2">
       <c r="N166" s="7"/>
       <c r="O166" s="7"/>
     </row>
-    <row r="167" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:36" x14ac:dyDescent="0.2">
       <c r="N167" s="7"/>
       <c r="O167" s="7"/>
     </row>
-    <row r="168" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:36" x14ac:dyDescent="0.2">
       <c r="N168" s="7"/>
       <c r="O168" s="7"/>
     </row>
-    <row r="169" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:36" x14ac:dyDescent="0.2">
       <c r="N169" s="7"/>
       <c r="O169" s="7"/>
     </row>

</xml_diff>